<commit_message>
Updated results from USB reading
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
   <si>
     <t>Time (MS)</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Average rate</t>
+  </si>
+  <si>
+    <t>GH Time (MS)</t>
+  </si>
+  <si>
+    <t>Average Read Rate</t>
   </si>
 </sst>
 </file>
@@ -390,11 +396,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2053236688"/>
-        <c:axId val="-2053263200"/>
+        <c:axId val="-2121935744"/>
+        <c:axId val="-2121926032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2053236688"/>
+        <c:axId val="-2121935744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -437,7 +443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053263200"/>
+        <c:crossAx val="-2121926032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -445,7 +451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2053263200"/>
+        <c:axId val="-2121926032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +502,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053236688"/>
+        <c:crossAx val="-2121935744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -592,17 +598,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.0451373045128362"/>
-          <c:y val="0.0122464207024289"/>
-          <c:w val="0.935472113769712"/>
-          <c:h val="0.85554455358632"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -611,11 +607,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>USB!$E$1</c:f>
+              <c:f>Mac!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average rate</c:v>
+                  <c:v>Average Read Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -634,7 +630,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>USB!$A$2:$A$17</c:f>
+              <c:f>Mac!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -690,57 +686,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USB!$E$2:$E$17</c:f>
+              <c:f>Mac!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>7865.614286830897</c:v>
+                  <c:v>1.94240512133333E9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8124.308851050567</c:v>
+                  <c:v>2.84882663E9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8143.81955173432</c:v>
+                  <c:v>2.993561893E9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7901.328241216208</c:v>
+                  <c:v>3.52632742033333E9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9665.304517215316</c:v>
+                  <c:v>3.92999666033333E9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7093.079212283551</c:v>
+                  <c:v>4.61995857166667E9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11469.01217672527</c:v>
+                  <c:v>4.62940431666667E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8155.551904050475</c:v>
+                  <c:v>4.73680669566667E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9490.608342670393</c:v>
+                  <c:v>5.23642279066667E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7221.16180772373</c:v>
+                  <c:v>4.963221073E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11485.45977904972</c:v>
+                  <c:v>5.20101209633333E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11226.72857675742</c:v>
+                  <c:v>5.34747782933333E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8719.70472183178</c:v>
+                  <c:v>5.57694870066667E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10021.42910799594</c:v>
+                  <c:v>5.161055375E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9946.986766834043</c:v>
+                  <c:v>5.66345077633333E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9032.747430813968</c:v>
+                  <c:v>5.20783671433333E9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -756,11 +752,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1199071536"/>
-        <c:axId val="-1210597264"/>
+        <c:axId val="-2076768896"/>
+        <c:axId val="-2076766592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1199071536"/>
+        <c:axId val="-2076768896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +799,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1210597264"/>
+        <c:crossAx val="-2076766592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -811,7 +807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1210597264"/>
+        <c:axId val="-2076766592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -862,7 +858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1199071536"/>
+        <c:crossAx val="-2076768896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -967,11 +963,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>USB!$D$1</c:f>
+              <c:f>USB!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time(MS)</c:v>
+                  <c:v>Average rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1046,57 +1042,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USB!$D$2:$D$17</c:f>
+              <c:f>USB!$E$2:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>4603.781</c:v>
+                  <c:v>7865.614286830897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4583.879</c:v>
+                  <c:v>8124.308851050567</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9573.268</c:v>
+                  <c:v>8143.81955173432</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4783.434</c:v>
+                  <c:v>7901.328241216208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4684.808</c:v>
+                  <c:v>9665.304517215316</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7954.071</c:v>
+                  <c:v>7093.079212283551</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4464.621</c:v>
+                  <c:v>11469.01217672527</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4743.317</c:v>
+                  <c:v>8155.551904050475</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4500.941</c:v>
+                  <c:v>9490.608342670393</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9406.51</c:v>
+                  <c:v>7221.16180772373</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4699.212</c:v>
+                  <c:v>11485.45977904972</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4442.114</c:v>
+                  <c:v>11226.72857675742</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4688.968</c:v>
+                  <c:v>8719.70472183178</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5578.259</c:v>
+                  <c:v>10021.42910799594</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6585.235</c:v>
+                  <c:v>9946.986766834043</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4833.639</c:v>
+                  <c:v>9032.747430813968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1112,11 +1108,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1316922720"/>
-        <c:axId val="-1208907056"/>
+        <c:axId val="-2070100560"/>
+        <c:axId val="-2076594656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1316922720"/>
+        <c:axId val="-2070100560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1155,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1208907056"/>
+        <c:crossAx val="-2076594656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1167,7 +1163,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1208907056"/>
+        <c:axId val="-2076594656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1218,7 +1214,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1316922720"/>
+        <c:crossAx val="-2070100560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1314,17 +1310,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12509208223972"/>
-          <c:y val="0.199490740740741"/>
-          <c:w val="0.857919072615923"/>
-          <c:h val="0.636447944006999"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1333,11 +1319,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>USB!$C$1</c:f>
+              <c:f>USB!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time(MS)</c:v>
+                  <c:v>Average Read Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1412,57 +1398,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USB!$C$2:$C$17</c:f>
+              <c:f>USB!$J$2:$J$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>5255.542</c:v>
+                  <c:v>3.07798564333333E9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8078.493</c:v>
+                  <c:v>4.39953864433333E9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4860.509</c:v>
+                  <c:v>4.84708397633333E9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9147.352999999999</c:v>
+                  <c:v>5.03722922933333E9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4708.142</c:v>
+                  <c:v>5.03622287266667E9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8200.026</c:v>
+                  <c:v>4.887016246E9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4810.651</c:v>
+                  <c:v>4.37847373133333E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7684.764</c:v>
+                  <c:v>4.330417803E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5355.274</c:v>
+                  <c:v>4.40744758266667E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7727.762</c:v>
+                  <c:v>4.98475490433333E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4482.144</c:v>
+                  <c:v>5.15729540633333E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4801.658</c:v>
+                  <c:v>5.33384464433333E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4504.955</c:v>
+                  <c:v>5.396860668E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5231.976</c:v>
+                  <c:v>5.60671355766667E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4547.462</c:v>
+                  <c:v>5.29245085466667E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7883.769</c:v>
+                  <c:v>5.06560553033333E9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1478,11 +1464,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1144589760"/>
-        <c:axId val="-1144132864"/>
+        <c:axId val="-2080453008"/>
+        <c:axId val="-2083871184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1144589760"/>
+        <c:axId val="-2080453008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1144132864"/>
+        <c:crossAx val="-2083871184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1533,7 +1519,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1144132864"/>
+        <c:axId val="-2083871184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1584,7 +1570,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1144589760"/>
+        <c:crossAx val="-2080453008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1689,11 +1675,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>USB!$B$1</c:f>
+              <c:f>cdf!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time(MS)</c:v>
+                  <c:v>Average rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1712,7 +1698,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>USB!$A$2:$A$17</c:f>
+              <c:f>cdf!$A$2:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -1768,57 +1754,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>USB!$B$2:$B$17</c:f>
+              <c:f>cdf!$E$2:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>10137.386</c:v>
+                  <c:v>443705.2165965177</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6697.601</c:v>
+                  <c:v>652694.829446427</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4879.814</c:v>
+                  <c:v>876066.7717517838</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5975.537</c:v>
+                  <c:v>915014.3983245587</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6880.35</c:v>
+                  <c:v>976139.9110040898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6020.532</c:v>
+                  <c:v>1.03572609162326E6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4438.76</c:v>
+                  <c:v>1.12103203734721E6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6857.726</c:v>
+                  <c:v>1.13225736786789E6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6716.632</c:v>
+                  <c:v>1.1866731047803E6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4647.043</c:v>
+                  <c:v>1.24226106323995E6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4513.037</c:v>
+                  <c:v>1.29110594879456E6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4766.222</c:v>
+                  <c:v>1.28970849903653E6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8844.119</c:v>
+                  <c:v>1.27234810182901E6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4884.772</c:v>
+                  <c:v>1.21653956222446E6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4679.77</c:v>
+                  <c:v>1.22501966587484E6</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4695.5</c:v>
+                  <c:v>1.22751494529165E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1834,11 +1820,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1197193552"/>
-        <c:axId val="-1316831744"/>
+        <c:axId val="-2126288416"/>
+        <c:axId val="-2126291872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1197193552"/>
+        <c:axId val="-2126288416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1881,7 +1867,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1316831744"/>
+        <c:crossAx val="-2126291872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1889,7 +1875,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1316831744"/>
+        <c:axId val="-2126291872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1926,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1197193552"/>
+        <c:crossAx val="-2126288416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2045,11 +2031,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>cdf!$E$1</c:f>
+              <c:f>cdf!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average rate</c:v>
+                  <c:v>Average Read Rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2068,7 +2054,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>cdf!$A$2:$A$18</c:f>
+              <c:f>cdf!$A$2:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
@@ -2124,57 +2110,57 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>cdf!$E$2:$E$18</c:f>
+              <c:f>cdf!$K$2:$K$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>443705.2165965177</c:v>
+                  <c:v>1.1926999045E9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>652694.829446427</c:v>
+                  <c:v>1.26008962475E9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>876066.7717517838</c:v>
+                  <c:v>1.32136298775E9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>915014.3983245587</c:v>
+                  <c:v>1.32954346175E9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>976139.9110040898</c:v>
+                  <c:v>1.598857004E9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.03572609162326E6</c:v>
+                  <c:v>1.69930228825E9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.12103203734721E6</c:v>
+                  <c:v>1.74594944325E9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.13225736786789E6</c:v>
+                  <c:v>1.7557718325E9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1866731047803E6</c:v>
+                  <c:v>1.814286474E9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.24226106323995E6</c:v>
+                  <c:v>1.81668112275E9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.29110594879456E6</c:v>
+                  <c:v>1.81900208625E9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.28970849903653E6</c:v>
+                  <c:v>1.815787226E9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.27234810182901E6</c:v>
+                  <c:v>1.77654495825E9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.21653956222446E6</c:v>
+                  <c:v>1.73683042825E9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.22501966587484E6</c:v>
+                  <c:v>1.42310208075E9</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.22751494529165E6</c:v>
+                  <c:v>1.43892043875E9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,11 +2176,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1144436496"/>
-        <c:axId val="-1144978608"/>
+        <c:axId val="-2109799696"/>
+        <c:axId val="-2079009712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1144436496"/>
+        <c:axId val="-2109799696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,7 +2223,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1144978608"/>
+        <c:crossAx val="-2079009712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2245,7 +2231,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1144978608"/>
+        <c:axId val="-2079009712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2296,7 +2282,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1144436496"/>
+        <c:crossAx val="-2109799696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5713,6 +5699,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5720,16 +5736,81 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5750,46 +5831,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5802,72 +5853,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6142,12 +6128,15 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -6168,10 +6157,18 @@
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -6187,8 +6184,21 @@
         <v>120.012</v>
       </c>
       <c r="E2">
-        <f>52428800/AVERAGE(D2,C2,B2)</f>
+        <f t="shared" ref="E2:E17" si="0">52428800/AVERAGE(D2,C2,B2)</f>
         <v>434399.21784808801</v>
+      </c>
+      <c r="H2">
+        <v>1113965791</v>
+      </c>
+      <c r="I2">
+        <v>2444423032</v>
+      </c>
+      <c r="J2">
+        <v>2268826541</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(H2,I2,J2)</f>
+        <v>1942405121.3333333</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -6205,8 +6215,21 @@
         <v>80.188999999999993</v>
       </c>
       <c r="E3">
-        <f>52428800/AVERAGE(D3,C3,B3)</f>
+        <f t="shared" si="0"/>
         <v>709478.42286405072</v>
+      </c>
+      <c r="H3">
+        <v>2505957141</v>
+      </c>
+      <c r="I3">
+        <v>3011707036</v>
+      </c>
+      <c r="J3">
+        <v>3028815713</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K17" si="1">AVERAGE(H3,I3,J3)</f>
+        <v>2848826630</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -6223,8 +6246,21 @@
         <v>59.905000000000001</v>
       </c>
       <c r="E4">
-        <f>52428800/AVERAGE(D4,C4,B4)</f>
+        <f t="shared" si="0"/>
         <v>814491.22261923249</v>
+      </c>
+      <c r="H4">
+        <v>2723809853</v>
+      </c>
+      <c r="I4">
+        <v>3087376582</v>
+      </c>
+      <c r="J4">
+        <v>3169499244</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>2993561893</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -6241,8 +6277,21 @@
         <v>61.161000000000001</v>
       </c>
       <c r="E5">
-        <f>52428800/AVERAGE(D5,C5,B5)</f>
+        <f t="shared" si="0"/>
         <v>794945.87027059798</v>
+      </c>
+      <c r="H5">
+        <v>2999359267</v>
+      </c>
+      <c r="I5">
+        <v>3785017446</v>
+      </c>
+      <c r="J5">
+        <v>3794605548</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>3526327420.3333335</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -6259,8 +6308,21 @@
         <v>62.037999999999997</v>
       </c>
       <c r="E6">
-        <f>52428800/AVERAGE(D6,C6,B6)</f>
+        <f t="shared" si="0"/>
         <v>862760.41380974848</v>
+      </c>
+      <c r="H6">
+        <v>3289478197</v>
+      </c>
+      <c r="I6">
+        <v>4274086956</v>
+      </c>
+      <c r="J6">
+        <v>4226424828</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>3929996660.3333335</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -6277,8 +6339,21 @@
         <v>58.356999999999999</v>
       </c>
       <c r="E7">
-        <f>52428800/AVERAGE(D7,C7,B7)</f>
+        <f t="shared" si="0"/>
         <v>923584.263065179</v>
+      </c>
+      <c r="H7">
+        <v>4159915366</v>
+      </c>
+      <c r="I7">
+        <v>5212473902</v>
+      </c>
+      <c r="J7">
+        <v>4487486447</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>4619958571.666667</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -6295,8 +6370,21 @@
         <v>53.375999999999998</v>
       </c>
       <c r="E8">
-        <f>52428800/AVERAGE(D8,C8,B8)</f>
+        <f t="shared" si="0"/>
         <v>940185.18407823402</v>
+      </c>
+      <c r="H8">
+        <v>4131505122</v>
+      </c>
+      <c r="I8">
+        <v>5016309998</v>
+      </c>
+      <c r="J8">
+        <v>4740397830</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>4629404316.666667</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -6313,8 +6401,21 @@
         <v>53.991999999999997</v>
       </c>
       <c r="E9">
-        <f>52428800/AVERAGE(D9,C9,B9)</f>
+        <f t="shared" si="0"/>
         <v>922192.58077944606</v>
+      </c>
+      <c r="H9">
+        <v>3961375141</v>
+      </c>
+      <c r="I9">
+        <v>5478453500</v>
+      </c>
+      <c r="J9">
+        <v>4770591446</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>4736806695.666667</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -6331,8 +6432,21 @@
         <v>54.82</v>
       </c>
       <c r="E10">
-        <f>52428800/AVERAGE(D10,C10,B10)</f>
+        <f t="shared" si="0"/>
         <v>955712.59304268577</v>
+      </c>
+      <c r="H10">
+        <v>4430602816</v>
+      </c>
+      <c r="I10">
+        <v>6092829750</v>
+      </c>
+      <c r="J10">
+        <v>5185835806</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>5236422790.666667</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -6349,8 +6463,21 @@
         <v>57.831000000000003</v>
       </c>
       <c r="E11">
-        <f>52428800/AVERAGE(D11,C11,B11)</f>
+        <f t="shared" si="0"/>
         <v>885173.05419550906</v>
+      </c>
+      <c r="H11">
+        <v>4113138075</v>
+      </c>
+      <c r="I11">
+        <v>5544109975</v>
+      </c>
+      <c r="J11">
+        <v>5232415169</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>4963221073</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -6367,8 +6494,21 @@
         <v>64.86</v>
       </c>
       <c r="E12">
-        <f>52428800/AVERAGE(D12,C12,B12)</f>
+        <f t="shared" si="0"/>
         <v>847800.0032341003</v>
+      </c>
+      <c r="H12">
+        <v>4105622552</v>
+      </c>
+      <c r="I12">
+        <v>5856875814</v>
+      </c>
+      <c r="J12">
+        <v>5640537923</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>5201012096.333333</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -6385,8 +6525,21 @@
         <v>59.96</v>
       </c>
       <c r="E13">
-        <f>52428800/AVERAGE(D13,C13,B13)</f>
+        <f t="shared" si="0"/>
         <v>841905.12894626975</v>
+      </c>
+      <c r="H13">
+        <v>4572279069</v>
+      </c>
+      <c r="I13">
+        <v>5627420393</v>
+      </c>
+      <c r="J13">
+        <v>5842734026</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>5347477829.333333</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -6403,8 +6556,21 @@
         <v>65.132000000000005</v>
       </c>
       <c r="E14">
-        <f>52428800/AVERAGE(D14,C14,B14)</f>
+        <f t="shared" si="0"/>
         <v>784924.94410731387</v>
+      </c>
+      <c r="H14">
+        <v>5019511728</v>
+      </c>
+      <c r="I14">
+        <v>5661857451</v>
+      </c>
+      <c r="J14">
+        <v>6049476923</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>5576948700.666667</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -6421,8 +6587,21 @@
         <v>68.075000000000003</v>
       </c>
       <c r="E15">
-        <f>52428800/AVERAGE(D15,C15,B15)</f>
+        <f t="shared" si="0"/>
         <v>770887.06238696666</v>
+      </c>
+      <c r="H15">
+        <v>3537705802</v>
+      </c>
+      <c r="I15">
+        <v>5937576443</v>
+      </c>
+      <c r="J15">
+        <v>6007883880</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>5161055375</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -6439,11 +6618,24 @@
         <v>68.518000000000001</v>
       </c>
       <c r="E16">
-        <f>52428800/AVERAGE(D16,C16,B16)</f>
+        <f t="shared" si="0"/>
         <v>722289.11513080855</v>
       </c>
+      <c r="H16">
+        <v>5092646915</v>
+      </c>
+      <c r="I16">
+        <v>5931978125</v>
+      </c>
+      <c r="J16">
+        <v>5965727289</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>5663450776.333333</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -6457,8 +6649,21 @@
         <v>65.311000000000007</v>
       </c>
       <c r="E17">
-        <f>52428800/AVERAGE(D17,C17,B17)</f>
+        <f t="shared" si="0"/>
         <v>745517.9736083725</v>
+      </c>
+      <c r="H17">
+        <v>4656888230</v>
+      </c>
+      <c r="I17">
+        <v>5297622094</v>
+      </c>
+      <c r="J17">
+        <v>5668999819</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>5207836714.333333</v>
       </c>
     </row>
   </sheetData>
@@ -6470,15 +6675,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6494,8 +6705,20 @@
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6512,8 +6735,21 @@
         <f>52428800/AVERAGE(B2,D2,C2)</f>
         <v>7865.6142868308971</v>
       </c>
+      <c r="G2">
+        <v>2734464534</v>
+      </c>
+      <c r="H2">
+        <v>3240346106</v>
+      </c>
+      <c r="I2">
+        <v>3259146290</v>
+      </c>
+      <c r="J2">
+        <f>AVERAGE(G2,H2,I2)</f>
+        <v>3077985643.3333335</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6530,8 +6766,21 @@
         <f t="shared" ref="E3:E17" si="0">52428800/AVERAGE(B3,D3,C3)</f>
         <v>8124.3088510505677</v>
       </c>
+      <c r="G3">
+        <v>4366640755</v>
+      </c>
+      <c r="H3">
+        <v>4418157303</v>
+      </c>
+      <c r="I3">
+        <v>4413817875</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J17" si="1">AVERAGE(G3,H3,I3)</f>
+        <v>4399538644.333333</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6548,8 +6797,21 @@
         <f t="shared" si="0"/>
         <v>8143.8195517343192</v>
       </c>
+      <c r="G4">
+        <v>4965632202</v>
+      </c>
+      <c r="H4">
+        <v>4760484261</v>
+      </c>
+      <c r="I4">
+        <v>4815135466</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>4847083976.333333</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6566,8 +6828,21 @@
         <f t="shared" si="0"/>
         <v>7901.3282412162089</v>
       </c>
+      <c r="G5">
+        <v>5228936170</v>
+      </c>
+      <c r="H5">
+        <v>4868040854</v>
+      </c>
+      <c r="I5">
+        <v>5014710664</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>5037229229.333333</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -6584,8 +6859,21 @@
         <f t="shared" si="0"/>
         <v>9665.3045172153161</v>
       </c>
+      <c r="G6">
+        <v>5198691125</v>
+      </c>
+      <c r="H6">
+        <v>4804105070</v>
+      </c>
+      <c r="I6">
+        <v>5105872423</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>5036222872.666667</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6602,8 +6890,21 @@
         <f t="shared" si="0"/>
         <v>7093.079212283551</v>
       </c>
+      <c r="G7">
+        <v>4863525046</v>
+      </c>
+      <c r="H7">
+        <v>4908297706</v>
+      </c>
+      <c r="I7">
+        <v>4889225986</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>4887016246</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -6620,8 +6921,21 @@
         <f t="shared" si="0"/>
         <v>11469.012176725269</v>
       </c>
+      <c r="G8">
+        <v>4622671565</v>
+      </c>
+      <c r="H8">
+        <v>4440609824</v>
+      </c>
+      <c r="I8">
+        <v>4072139805</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>4378473731.333333</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6638,8 +6952,21 @@
         <f t="shared" si="0"/>
         <v>8155.551904050476</v>
       </c>
+      <c r="G9">
+        <v>4617243505</v>
+      </c>
+      <c r="H9">
+        <v>4467729015</v>
+      </c>
+      <c r="I9">
+        <v>3906280889</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>4330417803</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6656,8 +6983,21 @@
         <f t="shared" si="0"/>
         <v>9490.6083426703935</v>
       </c>
+      <c r="G10">
+        <v>4749702551</v>
+      </c>
+      <c r="H10">
+        <v>4438103837</v>
+      </c>
+      <c r="I10">
+        <v>4034536360</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>4407447582.666667</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -6674,8 +7014,21 @@
         <f t="shared" si="0"/>
         <v>7221.1618077237308</v>
       </c>
+      <c r="G11">
+        <v>5281611820</v>
+      </c>
+      <c r="H11">
+        <v>5145122669</v>
+      </c>
+      <c r="I11">
+        <v>4527530224</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>4984754904.333333</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -6692,8 +7045,21 @@
         <f t="shared" si="0"/>
         <v>11485.459779049719</v>
       </c>
+      <c r="G12">
+        <v>5525606885</v>
+      </c>
+      <c r="H12">
+        <v>5171343087</v>
+      </c>
+      <c r="I12">
+        <v>4774936247</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>5157295406.333333</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -6710,8 +7076,21 @@
         <f t="shared" si="0"/>
         <v>11226.728576757421</v>
       </c>
+      <c r="G13">
+        <v>5890876404</v>
+      </c>
+      <c r="H13">
+        <v>5014710664</v>
+      </c>
+      <c r="I13">
+        <v>5095946865</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>5333844644.333333</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -6728,8 +7107,21 @@
         <f t="shared" si="0"/>
         <v>8719.7047218317821</v>
       </c>
+      <c r="G14">
+        <v>5624401930</v>
+      </c>
+      <c r="H14">
+        <v>5227198404</v>
+      </c>
+      <c r="I14">
+        <v>5338981670</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>5396860668</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -6746,8 +7138,21 @@
         <f t="shared" si="0"/>
         <v>10021.42910799594</v>
       </c>
+      <c r="G15">
+        <v>5792170870</v>
+      </c>
+      <c r="H15">
+        <v>5515917937</v>
+      </c>
+      <c r="I15">
+        <v>5512051866</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>5606713557.666667</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -6764,8 +7169,21 @@
         <f t="shared" si="0"/>
         <v>9946.986766834043</v>
       </c>
+      <c r="G16">
+        <v>5815729339</v>
+      </c>
+      <c r="H16">
+        <v>5390212474</v>
+      </c>
+      <c r="I16">
+        <v>4671410751</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>5292450854.666667</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -6781,6 +7199,19 @@
       <c r="E17">
         <f t="shared" si="0"/>
         <v>9032.7474308139681</v>
+      </c>
+      <c r="G17">
+        <v>5594394451</v>
+      </c>
+      <c r="H17">
+        <v>4716233883</v>
+      </c>
+      <c r="I17">
+        <v>4886188257</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>5065605530.333333</v>
       </c>
     </row>
   </sheetData>
@@ -6792,19 +7223,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -6821,8 +7256,20 @@
         <v>19</v>
       </c>
       <c r="F1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6839,8 +7286,21 @@
         <f>52428800/AVERAGE(B2,C2,D2)</f>
         <v>443705.21659651771</v>
       </c>
+      <c r="H2">
+        <v>1566987795</v>
+      </c>
+      <c r="I2">
+        <v>1605372799</v>
+      </c>
+      <c r="J2">
+        <v>1598439024</v>
+      </c>
+      <c r="K2">
+        <f>AVERAGE(H2,I2,J2,)</f>
+        <v>1192699904.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -6857,8 +7317,21 @@
         <f t="shared" ref="E3:E17" si="0">52428800/AVERAGE(B3,C3,D3)</f>
         <v>652694.82944642706</v>
       </c>
+      <c r="H3">
+        <v>1745105958</v>
+      </c>
+      <c r="I3">
+        <v>1752397080</v>
+      </c>
+      <c r="J3">
+        <v>1542855461</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K17" si="1">AVERAGE(H3,I3,J3,)</f>
+        <v>1260089624.75</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -6875,8 +7348,21 @@
         <f t="shared" si="0"/>
         <v>876066.77175178379</v>
       </c>
+      <c r="H4">
+        <v>1776043360</v>
+      </c>
+      <c r="I4">
+        <v>1764883303</v>
+      </c>
+      <c r="J4">
+        <v>1744525288</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>1321362987.75</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -6893,8 +7379,21 @@
         <f t="shared" si="0"/>
         <v>915014.39832455874</v>
       </c>
+      <c r="H5">
+        <v>1750057301</v>
+      </c>
+      <c r="I5">
+        <v>1780466379</v>
+      </c>
+      <c r="J5">
+        <v>1787650167</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>1329543461.75</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -6911,8 +7410,21 @@
         <f t="shared" si="0"/>
         <v>976139.91100408987</v>
       </c>
+      <c r="H6">
+        <v>2149749197</v>
+      </c>
+      <c r="I6">
+        <v>2121335221</v>
+      </c>
+      <c r="J6">
+        <v>2124343598</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>1598857004</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6929,8 +7441,21 @@
         <f t="shared" si="0"/>
         <v>1035726.0916232609</v>
       </c>
+      <c r="H7">
+        <v>2266701253</v>
+      </c>
+      <c r="I7">
+        <v>2258239770</v>
+      </c>
+      <c r="J7">
+        <v>2272268130</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>1699302288.25</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -6947,8 +7472,21 @@
         <f t="shared" si="0"/>
         <v>1121032.0373472078</v>
       </c>
+      <c r="H8">
+        <v>2323113507</v>
+      </c>
+      <c r="I8">
+        <v>2329133718</v>
+      </c>
+      <c r="J8">
+        <v>2331550548</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>1745949443.25</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6965,8 +7503,21 @@
         <f t="shared" si="0"/>
         <v>1132257.3678678893</v>
       </c>
+      <c r="H9">
+        <v>2363076923</v>
+      </c>
+      <c r="I9">
+        <v>2294979207</v>
+      </c>
+      <c r="J9">
+        <v>2365031200</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>1755771832.5</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -6983,8 +7534,21 @@
         <f t="shared" si="0"/>
         <v>1186673.1047802996</v>
       </c>
+      <c r="H10">
+        <v>2422212982</v>
+      </c>
+      <c r="I10">
+        <v>2416816226</v>
+      </c>
+      <c r="J10">
+        <v>2418116688</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>1814286474</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -7001,8 +7565,21 @@
         <f t="shared" si="0"/>
         <v>1242261.0632399519</v>
       </c>
+      <c r="H11">
+        <v>2419046447</v>
+      </c>
+      <c r="I11">
+        <v>2414034226</v>
+      </c>
+      <c r="J11">
+        <v>2433643818</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>1816681122.75</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -7019,8 +7596,21 @@
         <f t="shared" si="0"/>
         <v>1291105.9487945626</v>
       </c>
+      <c r="H12">
+        <v>2424453179</v>
+      </c>
+      <c r="I12">
+        <v>2431950521</v>
+      </c>
+      <c r="J12">
+        <v>2419604645</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>1819002086.25</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -7037,8 +7627,21 @@
         <f t="shared" si="0"/>
         <v>1289708.49903653</v>
       </c>
+      <c r="H13">
+        <v>2404623146</v>
+      </c>
+      <c r="I13">
+        <v>2438548837</v>
+      </c>
+      <c r="J13">
+        <v>2419976921</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>1815787226</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -7055,8 +7658,21 @@
         <f t="shared" si="0"/>
         <v>1272348.1018290068</v>
       </c>
+      <c r="H14">
+        <v>2377184311</v>
+      </c>
+      <c r="I14">
+        <v>2350013446</v>
+      </c>
+      <c r="J14">
+        <v>2378982076</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>1776544958.25</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -7073,8 +7689,21 @@
         <f t="shared" si="0"/>
         <v>1216539.5622244566</v>
       </c>
+      <c r="H15">
+        <v>2329133718</v>
+      </c>
+      <c r="I15">
+        <v>2298500657</v>
+      </c>
+      <c r="J15">
+        <v>2319687338</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>1736830428.25</v>
+      </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -7091,8 +7720,21 @@
         <f t="shared" si="0"/>
         <v>1225019.6658748395</v>
       </c>
+      <c r="H16">
+        <v>1910902684</v>
+      </c>
+      <c r="I16">
+        <v>1894446251</v>
+      </c>
+      <c r="J16">
+        <v>1887059388</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>1423102080.75</v>
+      </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -7108,6 +7750,19 @@
       <c r="E17">
         <f t="shared" si="0"/>
         <v>1227514.9452916477</v>
+      </c>
+      <c r="H17">
+        <v>1921055267</v>
+      </c>
+      <c r="I17">
+        <v>1895930568</v>
+      </c>
+      <c r="J17">
+        <v>1938695920</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>1438920438.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>